<commit_message>
klarer å trykke på alt utenon søkefeltKartButton
</commit_message>
<xml_diff>
--- a/travelResults.xlsx
+++ b/travelResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vquach\projects\FinnTraining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{471A7B2F-5E97-47B4-8B33-CB2A27795BC2}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{CAA8FCB6-DF3E-4810-A062-68E96AB5768B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
     <workbookView windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
@@ -25,12 +25,144 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
-  <si>
-    <t>m</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="46">
   <si>
     <t>Søk</t>
+  </si>
+  <si>
+    <t>to. 16.11</t>
+  </si>
+  <si>
+    <t>fr. 17.11</t>
+  </si>
+  <si>
+    <t>lø. 18.11</t>
+  </si>
+  <si>
+    <t>sø. 19.11</t>
+  </si>
+  <si>
+    <t>ma. 20.11</t>
+  </si>
+  <si>
+    <t>ti. 21.11</t>
+  </si>
+  <si>
+    <t>981 kr</t>
+  </si>
+  <si>
+    <t>1 048 kr</t>
+  </si>
+  <si>
+    <t>841 kr</t>
+  </si>
+  <si>
+    <t>976 kr</t>
+  </si>
+  <si>
+    <t>1 044 kr</t>
+  </si>
+  <si>
+    <t>856 kr</t>
+  </si>
+  <si>
+    <t>816 kr</t>
+  </si>
+  <si>
+    <t>752 kr</t>
+  </si>
+  <si>
+    <t>on. 22.11</t>
+  </si>
+  <si>
+    <t>826 kr</t>
+  </si>
+  <si>
+    <t>1 118 kr</t>
+  </si>
+  <si>
+    <t>998 kr</t>
+  </si>
+  <si>
+    <t>837 kr</t>
+  </si>
+  <si>
+    <t>798 kr</t>
+  </si>
+  <si>
+    <t>to. 23.11</t>
+  </si>
+  <si>
+    <t>1 093 kr</t>
+  </si>
+  <si>
+    <t>944 kr</t>
+  </si>
+  <si>
+    <t>853 kr</t>
+  </si>
+  <si>
+    <t>fr. 24.11</t>
+  </si>
+  <si>
+    <t>1 196 kr</t>
+  </si>
+  <si>
+    <t>1 025 kr</t>
+  </si>
+  <si>
+    <t>1 046 kr</t>
+  </si>
+  <si>
+    <t>835 kr</t>
+  </si>
+  <si>
+    <t>lø. 25.11</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>1 270 kr</t>
+  </si>
+  <si>
+    <t>1 143 kr</t>
+  </si>
+  <si>
+    <t>1 027 kr</t>
+  </si>
+  <si>
+    <t>797 kr</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>1 218 kr</t>
+  </si>
+  <si>
+    <t>1 010 kr</t>
+  </si>
+  <si>
+    <t>1 358 kr</t>
+  </si>
+  <si>
+    <t>1 011 kr</t>
+  </si>
+  <si>
+    <t>1 129 kr</t>
+  </si>
+  <si>
+    <t>sø. 26.11</t>
+  </si>
+  <si>
+    <t>1 214 kr</t>
+  </si>
+  <si>
+    <t>ma. 27.11</t>
   </si>
 </sst>
 </file>
@@ -349,45 +481,227 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
       <c r="F6" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>